<commit_message>
mise en place d'onglets
</commit_message>
<xml_diff>
--- a/Datas/Log/Log_export.xlsx
+++ b/Datas/Log/Log_export.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,7 +522,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>11821</v>
+        <v>11691</v>
       </c>
       <c r="B2" t="n">
         <v>1280</v>
@@ -532,17 +532,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Sébastien</t>
+          <t>Romain</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>GUYENNET</t>
+          <t>COUPPE</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Sebastien.GUYENNET@fr.toyota-industries.eu</t>
+          <t>Romain.Couppe@fr.toyota-industries.eu</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -577,16 +577,16 @@
         <v>6</v>
       </c>
       <c r="N2" t="n">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>2025-09-01 13:30</t>
+          <t>2025-09-03 13:30</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>2025-09-02 17:30</t>
+          <t>2025-09-04 17:30</t>
         </is>
       </c>
       <c r="Q2" t="n">
@@ -595,7 +595,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>11672</v>
+        <v>11628</v>
       </c>
       <c r="B3" t="n">
         <v>1280</v>
@@ -605,17 +605,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Steven</t>
+          <t>Michel</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>BODINEAU</t>
+          <t>LAUTRIDOU</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Steven.Bodineau@fr.toyota-industries.eu</t>
+          <t>Michel.Lautridou@fr.toyota-industries.eu</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -650,16 +650,16 @@
         <v>6</v>
       </c>
       <c r="N3" t="n">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>2025-09-01 13:30</t>
+          <t>2025-09-03 13:30</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>2025-09-02 17:30</t>
+          <t>2025-09-04 17:30</t>
         </is>
       </c>
       <c r="Q3" t="n">
@@ -668,7 +668,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>11027</v>
+        <v>11786</v>
       </c>
       <c r="B4" t="n">
         <v>1280</v>
@@ -678,17 +678,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>François-Xavier</t>
+          <t>Stéphane</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>LUBERT</t>
+          <t>VILLETTE</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Francois-Xavier.Lubert@fr.toyota-industries.eu</t>
+          <t>Stephane.VILLETTE@fr.toyota-industries.eu</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -723,16 +723,16 @@
         <v>6</v>
       </c>
       <c r="N4" t="n">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>2025-09-01 13:30</t>
+          <t>2025-09-03 13:30</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>2025-09-02 17:30</t>
+          <t>2025-09-04 17:30</t>
         </is>
       </c>
       <c r="Q4" t="n">
@@ -741,7 +741,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>11368</v>
+        <v>11929</v>
       </c>
       <c r="B5" t="n">
         <v>1280</v>
@@ -751,22 +751,22 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Rémi</t>
+          <t>Hervé</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>BOIZUMEAU</t>
+          <t>GUION</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>r.boizumeau@clenet-manutentionindustrie.fr</t>
+          <t>Herve.GUION@fr.toyota-industries.eu</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>CMI</t>
+          <t>Toyota Material Handling France S.A.S.</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -796,19 +796,165 @@
         <v>6</v>
       </c>
       <c r="N5" t="n">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>2025-09-01 13:30</t>
+          <t>2025-09-03 13:30</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>2025-09-02 17:30</t>
+          <t>2025-09-04 17:30</t>
         </is>
       </c>
       <c r="Q5" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>11712</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1280</v>
+      </c>
+      <c r="C6" t="n">
+        <v>300</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Guillaume</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>TREBUTIEN</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Guillaume.TREBUTIEN@fr.toyota-industries.eu</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Toyota Material Handling France S.A.S.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>LITHIUM-ION TMHMS &amp; TMHMI</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>LITHIUM-ION TMHMS &amp; TMHMI</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>1404-T2-TE-61</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>719</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>CARQUEFOU 2025 - LITHIUM-ION TMHMS &amp; TMHMI</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>6</v>
+      </c>
+      <c r="N6" t="n">
+        <v>2012</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>2025-09-03 13:30</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>2025-09-04 17:30</t>
+        </is>
+      </c>
+      <c r="Q6" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>15809</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1280</v>
+      </c>
+      <c r="C7" t="n">
+        <v>300</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Jean-Jacques</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>MUGABE</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Jean-Jacques.MUGABE@fr.toyota-industries.eu</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Toyota Material Handling France S.A.S.</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>LITHIUM-ION TMHMS &amp; TMHMI</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>LITHIUM-ION TMHMS &amp; TMHMI</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>1404-T2-TE-61</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>719</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>CARQUEFOU 2025 - LITHIUM-ION TMHMS &amp; TMHMI</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>6</v>
+      </c>
+      <c r="N7" t="n">
+        <v>2012</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>2025-09-03 13:30</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>2025-09-04 17:30</t>
+        </is>
+      </c>
+      <c r="Q7" t="n">
         <v>12</v>
       </c>
     </row>

</xml_diff>